<commit_message>
update al but NW traverse that needs to be re-evaluated in the code
</commit_message>
<xml_diff>
--- a/planning_info/Swiss_Camp_2021_July_16-23.xlsx
+++ b/planning_info/Swiss_Camp_2021_July_16-23.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="48">
   <si>
     <t>date</t>
   </si>
@@ -43,7 +43,7 @@
     <t>distance (nm)</t>
   </si>
   <si>
-    <t>fly time (h)</t>
+    <t>fly+taxi+circle time (h)</t>
   </si>
   <si>
     <t>arrival time (local time)</t>
@@ -115,6 +115,12 @@
     <t>SWC</t>
   </si>
   <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>total fly time no taxi or circling</t>
+  </si>
+  <si>
     <t>Ilulissat</t>
   </si>
   <si>
@@ -122,6 +128,9 @@
   </si>
   <si>
     <t>put in full load to Swiss Camp. first arrival after 1 year. PAX names: Derek Houtz. Jason Box. Simon Steffen. nn1</t>
+  </si>
+  <si>
+    <t>return empty to JAV</t>
   </si>
   <si>
     <t>put in with 1 PAX remaining gear</t>
@@ -506,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -599,14 +608,14 @@
       <c r="H2">
         <v>4</v>
       </c>
-      <c r="I2">
-        <v>42</v>
+      <c r="I2" t="s">
+        <v>33</v>
       </c>
       <c r="J2">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K2">
-        <v>9.199999999999999</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="L2">
         <v>0.5</v>
@@ -624,16 +633,16 @@
         <v>-49.3158</v>
       </c>
       <c r="Q2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S2">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -659,16 +668,16 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>42</v>
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
       </c>
       <c r="J3">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K3">
-        <v>10.4</v>
+        <v>10.6</v>
       </c>
       <c r="L3">
         <v>0.5</v>
@@ -686,78 +695,24 @@
         <v>-51.0664</v>
       </c>
       <c r="Q3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3">
+        <v>105</v>
+      </c>
+      <c r="T3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="I4" t="s">
         <v>34</v>
       </c>
-      <c r="R3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3">
-        <v>130</v>
-      </c>
-      <c r="T3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4">
-        <v>250</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>42</v>
-      </c>
       <c r="J4">
-        <v>0.72</v>
-      </c>
-      <c r="K4">
-        <v>13.7</v>
-      </c>
-      <c r="L4">
-        <v>0.5</v>
-      </c>
-      <c r="M4">
-        <v>69.2405</v>
-      </c>
-      <c r="N4">
-        <v>-51.0664</v>
-      </c>
-      <c r="O4">
-        <v>69.56829999999999</v>
-      </c>
-      <c r="P4">
-        <v>-49.3158</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4">
-        <v>130</v>
-      </c>
-      <c r="T4" t="s">
-        <v>36</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -774,176 +729,122 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5">
         <v>250</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>42</v>
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
       </c>
       <c r="J5">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K5">
-        <v>14.9</v>
+        <v>13.8</v>
       </c>
       <c r="L5">
         <v>0.5</v>
       </c>
       <c r="M5">
-        <v>69.56829999999999</v>
+        <v>69.2405</v>
       </c>
       <c r="N5">
-        <v>-49.3158</v>
+        <v>-51.0664</v>
       </c>
       <c r="O5">
-        <v>69.2405</v>
+        <v>69.56829999999999</v>
       </c>
       <c r="P5">
-        <v>-51.0664</v>
+        <v>-49.3158</v>
       </c>
       <c r="Q5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S5">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>8.25</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>42</v>
+      <c r="I6" t="s">
+        <v>33</v>
       </c>
       <c r="J6">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K6">
-        <v>9</v>
+        <v>15.1</v>
       </c>
       <c r="L6">
         <v>0.5</v>
       </c>
       <c r="M6">
-        <v>69.2405</v>
+        <v>69.56829999999999</v>
       </c>
       <c r="N6">
-        <v>-51.0664</v>
+        <v>-49.3158</v>
       </c>
       <c r="O6">
-        <v>69.56829999999999</v>
+        <v>69.2405</v>
       </c>
       <c r="P6">
-        <v>-49.3158</v>
+        <v>-51.0664</v>
       </c>
       <c r="Q6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6">
+        <v>105</v>
+      </c>
+      <c r="T6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="I7" t="s">
         <v>34</v>
       </c>
-      <c r="S6">
-        <v>130</v>
-      </c>
-      <c r="T6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>8.25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7">
-        <v>450</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>42</v>
-      </c>
       <c r="J7">
-        <v>0.72</v>
-      </c>
-      <c r="K7">
-        <v>10.2</v>
-      </c>
-      <c r="L7">
-        <v>0.5</v>
-      </c>
-      <c r="M7">
-        <v>69.56829999999999</v>
-      </c>
-      <c r="N7">
-        <v>-49.3158</v>
-      </c>
-      <c r="O7">
-        <v>69.2405</v>
-      </c>
-      <c r="P7">
-        <v>-51.0664</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" t="s">
-        <v>33</v>
-      </c>
-      <c r="S7">
-        <v>130</v>
-      </c>
-      <c r="T7" t="s">
-        <v>38</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -971,14 +872,14 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8">
-        <v>42</v>
+      <c r="I8" t="s">
+        <v>33</v>
       </c>
       <c r="J8">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K8">
-        <v>11.4</v>
+        <v>9.1</v>
       </c>
       <c r="L8">
         <v>0.5</v>
@@ -996,16 +897,16 @@
         <v>-49.3158</v>
       </c>
       <c r="Q8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S8">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1033,14 +934,14 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9">
-        <v>42</v>
+      <c r="I9" t="s">
+        <v>33</v>
       </c>
       <c r="J9">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K9">
-        <v>12.6</v>
+        <v>10.4</v>
       </c>
       <c r="L9">
         <v>0.5</v>
@@ -1058,16 +959,16 @@
         <v>-51.0664</v>
       </c>
       <c r="Q9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S9">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1095,14 +996,14 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10">
-        <v>42</v>
+      <c r="I10" t="s">
+        <v>33</v>
       </c>
       <c r="J10">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K10">
-        <v>13.9</v>
+        <v>11.7</v>
       </c>
       <c r="L10">
         <v>0.5</v>
@@ -1120,16 +1021,16 @@
         <v>-49.3158</v>
       </c>
       <c r="Q10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S10">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1157,14 +1058,14 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11">
-        <v>42</v>
+      <c r="I11" t="s">
+        <v>33</v>
       </c>
       <c r="J11">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K11">
-        <v>15.1</v>
+        <v>13</v>
       </c>
       <c r="L11">
         <v>0.5</v>
@@ -1182,16 +1083,16 @@
         <v>-51.0664</v>
       </c>
       <c r="Q11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S11">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1219,14 +1120,14 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
-        <v>42</v>
+      <c r="I12" t="s">
+        <v>33</v>
       </c>
       <c r="J12">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K12">
-        <v>16.3</v>
+        <v>14.3</v>
       </c>
       <c r="L12">
         <v>0.5</v>
@@ -1244,16 +1145,16 @@
         <v>-49.3158</v>
       </c>
       <c r="Q12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S12">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1281,14 +1182,14 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
-        <v>42</v>
+      <c r="I13" t="s">
+        <v>33</v>
       </c>
       <c r="J13">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K13">
-        <v>17.5</v>
+        <v>15.6</v>
       </c>
       <c r="L13">
         <v>0.5</v>
@@ -1306,30 +1207,30 @@
         <v>-51.0664</v>
       </c>
       <c r="Q13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S13">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>8.5</v>
+        <v>8.25</v>
       </c>
       <c r="E14" t="s">
         <v>31</v>
@@ -1338,19 +1239,19 @@
         <v>32</v>
       </c>
       <c r="G14">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>33</v>
       </c>
       <c r="J14">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K14">
-        <v>9.199999999999999</v>
+        <v>16.9</v>
       </c>
       <c r="L14">
         <v>0.5</v>
@@ -1368,30 +1269,30 @@
         <v>-49.3158</v>
       </c>
       <c r="Q14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S14">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>8.5</v>
+        <v>8.25</v>
       </c>
       <c r="E15" t="s">
         <v>32</v>
@@ -1400,19 +1301,19 @@
         <v>31</v>
       </c>
       <c r="G15">
-        <v>200</v>
+        <v>450</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15">
-        <v>42</v>
+      <c r="I15" t="s">
+        <v>33</v>
       </c>
       <c r="J15">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K15">
-        <v>10.4</v>
+        <v>18.2</v>
       </c>
       <c r="L15">
         <v>0.5</v>
@@ -1430,275 +1331,167 @@
         <v>-51.0664</v>
       </c>
       <c r="Q15" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" t="s">
+        <v>35</v>
+      </c>
+      <c r="S15">
+        <v>105</v>
+      </c>
+      <c r="T15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="I16" t="s">
         <v>34</v>
       </c>
-      <c r="R15" t="s">
-        <v>33</v>
-      </c>
-      <c r="S15">
-        <v>130</v>
-      </c>
-      <c r="T15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>8.5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16">
-        <v>100</v>
-      </c>
-      <c r="H16">
-        <v>5</v>
-      </c>
-      <c r="I16">
-        <v>42</v>
-      </c>
       <c r="J16">
-        <v>0.72</v>
-      </c>
-      <c r="K16">
-        <v>9.199999999999999</v>
-      </c>
-      <c r="L16">
-        <v>1.5</v>
-      </c>
-      <c r="M16">
-        <v>69.2405</v>
-      </c>
-      <c r="N16">
-        <v>-51.0664</v>
-      </c>
-      <c r="O16">
-        <v>69.56829999999999</v>
-      </c>
-      <c r="P16">
-        <v>-49.3158</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>33</v>
-      </c>
-      <c r="R16" t="s">
-        <v>34</v>
-      </c>
-      <c r="S16">
-        <v>130</v>
-      </c>
-      <c r="T16" t="s">
-        <v>43</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>8.5</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G17">
         <v>200</v>
       </c>
       <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>42</v>
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>33</v>
       </c>
       <c r="J17">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K17">
-        <v>11.4</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="L17">
         <v>0.5</v>
       </c>
       <c r="M17">
-        <v>69.56829999999999</v>
+        <v>69.2405</v>
       </c>
       <c r="N17">
-        <v>-49.3158</v>
+        <v>-51.0664</v>
       </c>
       <c r="O17">
-        <v>69.2405</v>
+        <v>69.56829999999999</v>
       </c>
       <c r="P17">
-        <v>-51.0664</v>
+        <v>-49.3158</v>
       </c>
       <c r="Q17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S17">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <v>8.5</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="I18">
-        <v>42</v>
+      <c r="I18" t="s">
+        <v>33</v>
       </c>
       <c r="J18">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K18">
-        <v>9.199999999999999</v>
+        <v>10.6</v>
       </c>
       <c r="L18">
         <v>0.5</v>
       </c>
       <c r="M18">
-        <v>69.2405</v>
+        <v>69.56829999999999</v>
       </c>
       <c r="N18">
-        <v>-51.0664</v>
+        <v>-49.3158</v>
       </c>
       <c r="O18">
-        <v>69.56829999999999</v>
+        <v>69.2405</v>
       </c>
       <c r="P18">
-        <v>-49.3158</v>
+        <v>-51.0664</v>
       </c>
       <c r="Q18" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R18" t="s">
+        <v>35</v>
+      </c>
+      <c r="S18">
+        <v>105</v>
+      </c>
+      <c r="T18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="I19" t="s">
         <v>34</v>
       </c>
-      <c r="S18">
-        <v>130</v>
-      </c>
-      <c r="T18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>8.5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19">
-        <v>100</v>
-      </c>
-      <c r="H19">
-        <v>5</v>
-      </c>
-      <c r="I19">
-        <v>42</v>
-      </c>
       <c r="J19">
-        <v>0.72</v>
-      </c>
-      <c r="K19">
-        <v>10.4</v>
-      </c>
-      <c r="L19">
-        <v>0.5</v>
-      </c>
-      <c r="M19">
-        <v>69.56829999999999</v>
-      </c>
-      <c r="N19">
-        <v>-49.3158</v>
-      </c>
-      <c r="O19">
-        <v>69.2405</v>
-      </c>
-      <c r="P19">
-        <v>-51.0664</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>34</v>
-      </c>
-      <c r="R19" t="s">
-        <v>33</v>
-      </c>
-      <c r="S19">
-        <v>130</v>
-      </c>
-      <c r="T19" t="s">
-        <v>44</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>8.5</v>
@@ -1710,22 +1503,22 @@
         <v>32</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>42</v>
+        <v>5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>33</v>
       </c>
       <c r="J20">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K20">
-        <v>11.7</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="L20">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="M20">
         <v>69.2405</v>
@@ -1740,27 +1533,27 @@
         <v>-49.3158</v>
       </c>
       <c r="Q20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S20">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="T20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21">
         <v>8.5</v>
@@ -1772,19 +1565,19 @@
         <v>31</v>
       </c>
       <c r="G21">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="I21">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>33</v>
       </c>
       <c r="J21">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K21">
-        <v>12.9</v>
+        <v>11.6</v>
       </c>
       <c r="L21">
         <v>0.5</v>
@@ -1802,78 +1595,24 @@
         <v>-51.0664</v>
       </c>
       <c r="Q21" t="s">
+        <v>36</v>
+      </c>
+      <c r="R21" t="s">
+        <v>35</v>
+      </c>
+      <c r="S21">
+        <v>105</v>
+      </c>
+      <c r="T21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="I22" t="s">
         <v>34</v>
       </c>
-      <c r="R21" t="s">
-        <v>33</v>
-      </c>
-      <c r="S21">
-        <v>130</v>
-      </c>
-      <c r="T21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>8.5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>42</v>
-      </c>
       <c r="J22">
-        <v>0.72</v>
-      </c>
-      <c r="K22">
-        <v>14.1</v>
-      </c>
-      <c r="L22">
-        <v>0.5</v>
-      </c>
-      <c r="M22">
-        <v>69.2405</v>
-      </c>
-      <c r="N22">
-        <v>-51.0664</v>
-      </c>
-      <c r="O22">
-        <v>69.56829999999999</v>
-      </c>
-      <c r="P22">
-        <v>-49.3158</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>33</v>
-      </c>
-      <c r="R22" t="s">
-        <v>34</v>
-      </c>
-      <c r="S22">
-        <v>130</v>
-      </c>
-      <c r="T22" t="s">
-        <v>44</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -1890,52 +1629,370 @@
         <v>8.5</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G23">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>2</v>
-      </c>
-      <c r="I23">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>33</v>
       </c>
       <c r="J23">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="K23">
-        <v>15.3</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="L23">
         <v>0.5</v>
       </c>
       <c r="M23">
-        <v>69.56829999999999</v>
+        <v>69.2405</v>
       </c>
       <c r="N23">
-        <v>-49.3158</v>
+        <v>-51.0664</v>
       </c>
       <c r="O23">
-        <v>69.2405</v>
+        <v>69.56829999999999</v>
       </c>
       <c r="P23">
-        <v>-51.0664</v>
+        <v>-49.3158</v>
       </c>
       <c r="Q23" t="s">
+        <v>35</v>
+      </c>
+      <c r="R23" t="s">
+        <v>36</v>
+      </c>
+      <c r="S23">
+        <v>105</v>
+      </c>
+      <c r="T23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>8.5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24">
+        <v>0.8</v>
+      </c>
+      <c r="K24">
+        <v>10.6</v>
+      </c>
+      <c r="L24">
+        <v>0.5</v>
+      </c>
+      <c r="M24">
+        <v>69.56829999999999</v>
+      </c>
+      <c r="N24">
+        <v>-49.3158</v>
+      </c>
+      <c r="O24">
+        <v>69.2405</v>
+      </c>
+      <c r="P24">
+        <v>-51.0664</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>36</v>
+      </c>
+      <c r="R24" t="s">
+        <v>35</v>
+      </c>
+      <c r="S24">
+        <v>105</v>
+      </c>
+      <c r="T24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>8.5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25">
+        <v>0.8</v>
+      </c>
+      <c r="K25">
+        <v>11.9</v>
+      </c>
+      <c r="L25">
+        <v>0.5</v>
+      </c>
+      <c r="M25">
+        <v>69.2405</v>
+      </c>
+      <c r="N25">
+        <v>-51.0664</v>
+      </c>
+      <c r="O25">
+        <v>69.56829999999999</v>
+      </c>
+      <c r="P25">
+        <v>-49.3158</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>35</v>
+      </c>
+      <c r="R25" t="s">
+        <v>36</v>
+      </c>
+      <c r="S25">
+        <v>105</v>
+      </c>
+      <c r="T25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>8.5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26">
+        <v>0.8</v>
+      </c>
+      <c r="K26">
+        <v>13.2</v>
+      </c>
+      <c r="L26">
+        <v>0.5</v>
+      </c>
+      <c r="M26">
+        <v>69.56829999999999</v>
+      </c>
+      <c r="N26">
+        <v>-49.3158</v>
+      </c>
+      <c r="O26">
+        <v>69.2405</v>
+      </c>
+      <c r="P26">
+        <v>-51.0664</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>36</v>
+      </c>
+      <c r="R26" t="s">
+        <v>35</v>
+      </c>
+      <c r="S26">
+        <v>105</v>
+      </c>
+      <c r="T26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>8.5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27">
+        <v>0.8</v>
+      </c>
+      <c r="K27">
+        <v>14.5</v>
+      </c>
+      <c r="L27">
+        <v>0.5</v>
+      </c>
+      <c r="M27">
+        <v>69.2405</v>
+      </c>
+      <c r="N27">
+        <v>-51.0664</v>
+      </c>
+      <c r="O27">
+        <v>69.56829999999999</v>
+      </c>
+      <c r="P27">
+        <v>-49.3158</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>35</v>
+      </c>
+      <c r="R27" t="s">
+        <v>36</v>
+      </c>
+      <c r="S27">
+        <v>105</v>
+      </c>
+      <c r="T27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>8.5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28">
+        <v>100</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28">
+        <v>0.8</v>
+      </c>
+      <c r="K28">
+        <v>15.8</v>
+      </c>
+      <c r="L28">
+        <v>0.5</v>
+      </c>
+      <c r="M28">
+        <v>69.56829999999999</v>
+      </c>
+      <c r="N28">
+        <v>-49.3158</v>
+      </c>
+      <c r="O28">
+        <v>69.2405</v>
+      </c>
+      <c r="P28">
+        <v>-51.0664</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>36</v>
+      </c>
+      <c r="R28" t="s">
+        <v>35</v>
+      </c>
+      <c r="S28">
+        <v>105</v>
+      </c>
+      <c r="T28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="I29" t="s">
         <v>34</v>
       </c>
-      <c r="R23" t="s">
-        <v>33</v>
-      </c>
-      <c r="S23">
-        <v>130</v>
-      </c>
-      <c r="T23" t="s">
-        <v>44</v>
+      <c r="J29">
+        <v>2.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>